<commit_message>
Added Transaction Tab filtering function, a Delete Transaction Button, and fixed None type error when adding data to Transaction Table
</commit_message>
<xml_diff>
--- a/transactionsSpreadsheet.xlsx
+++ b/transactionsSpreadsheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -428,51 +428,46 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col width="16.5546875" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="16.5546875" customWidth="1" min="2" max="2"/>
-    <col width="9.5546875" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="38.33203125" customWidth="1" style="1" min="5" max="5"/>
+    <col width="16.5703125" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="16.5703125" customWidth="1" min="2" max="2"/>
+    <col width="9.5703125" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="38.28515625" customWidth="1" style="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Description</t>
+          <t>bought new bike</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>From Account</t>
+          <t>US Bank Checking</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Amount</t>
+          <t>15000.29</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Date</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Memo</t>
+          <t>01-01-2023</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>bye</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -482,7 +477,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2.35</t>
+          <t>80000</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -494,7 +489,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>bought new bike</t>
+          <t>new car 2</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -504,7 +499,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>15000.29</t>
+          <t>90000</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -516,7 +511,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>new car</t>
+          <t>mortgage</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -526,7 +521,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>80000</t>
+          <t>2000</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -538,17 +533,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>new car 2</t>
+          <t>Cell Phone</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>US Bank Checking</t>
+          <t>US Bank Savings</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>90000</t>
+          <t>699.99</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -560,17 +555,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>mortgage</t>
+          <t>Lawn Mower</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>US Bank Checking</t>
+          <t>Cash in wallet</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2000</t>
+          <t>459.79</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -582,51 +577,61 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Cell Phone</t>
+          <t>New windows</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>US Bank Savings</t>
+          <t>US Bank Checking</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>699.99</t>
+          <t>33575.84</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
           <t>01-01-2023</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Finally got my new windows!</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Lawn Mower</t>
+          <t>Tires for 4Runner</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Cash in wallet</t>
+          <t>US Bank Savings</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>459.79</t>
+          <t>1534.34</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
           <t>01-01-2023</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>35" tires!!</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>New windows</t>
+          <t>Lift for 4runner</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -636,7 +641,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>33575.84</t>
+          <t>6387.12</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -646,24 +651,24 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Finally got my new windows!</t>
+          <t>3" lift, Check!!</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Tires for 4Runner</t>
+          <t>Checking for Scroll</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>US Bank Savings</t>
+          <t>US Bank Checking</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1534.34</t>
+          <t>.01</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -673,24 +678,24 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>35" tires!!</t>
+          <t>will this work?</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Lift for 4runner</t>
+          <t>New Headphones</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>US Bank Checking</t>
+          <t>US Bank Savings</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>6387.12</t>
+          <t>235.69</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -700,24 +705,24 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>3" lift, Check!!</t>
+          <t>Music!!!</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Checking for Scroll</t>
+          <t>New Gun</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>US Bank Checking</t>
+          <t>US Bank Savings</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>.01</t>
+          <t>350.68</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -727,7 +732,181 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>will this work?</t>
+          <t>Bang, Bang</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Office Desk</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>US Bank Checking</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>608.79</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>01-01-2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Pens</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Cash in wallet</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>8.98</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>01-01-2023</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Ran out of pens and needed more.</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Powerwheel for Lucas</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>US Bank Checking</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>348.46</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>01-01-2023</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Love that kid!!</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>New computer</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>US Bank Checking</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>2300.98</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>01-01-2023</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Very powerfull</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Tire for dirtbike</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>US Bank Checking</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>97.87</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>01-01-2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>New bib for tire</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>US Bank Checking</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>120.35</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>01-01-2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Notebooks for work</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>US Bank Checking</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>18.59</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>03-24-2023</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Gotta keep your notes!</t>
         </is>
       </c>
     </row>
@@ -749,11 +928,11 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col width="15.44140625" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="14.33203125" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="8.88671875" customWidth="1" min="3" max="3"/>
+    <col width="15.42578125" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="14.28515625" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="8.85546875" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
Separated the Transaction tab code from main.py into its own transaction_tab.py file.
</commit_message>
<xml_diff>
--- a/transactionsSpreadsheet.xlsx
+++ b/transactionsSpreadsheet.xlsx
@@ -428,13 +428,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="16.5703125" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="16.5703125" customWidth="1" min="2" max="2"/>
@@ -761,17 +761,17 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Pens</t>
+          <t>Powerwheel for Lucas</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Cash in wallet</t>
+          <t>US Bank Checking</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>8.98</t>
+          <t>348.46</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -781,14 +781,14 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Ran out of pens and needed more.</t>
+          <t>Love that kid!!</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Powerwheel for Lucas</t>
+          <t>New computer</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -798,7 +798,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>348.46</t>
+          <t>2300.98</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -808,14 +808,14 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Love that kid!!</t>
+          <t>Very powerfull</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>New computer</t>
+          <t>Tire for dirtbike</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -825,24 +825,19 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2300.98</t>
+          <t>97.87</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
           <t>01-01-2023</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>Very powerfull</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Tire for dirtbike</t>
+          <t>New bib for tire</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -852,7 +847,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>97.87</t>
+          <t>120.35</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -864,7 +859,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>New bib for tire</t>
+          <t>Notebooks for work</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -874,37 +869,15 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>120.35</t>
+          <t>18.59</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>01-01-2023</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Notebooks for work</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>US Bank Checking</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>18.59</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
           <t>03-24-2023</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
+      <c r="E18" t="inlineStr">
         <is>
           <t>Gotta keep your notes!</t>
         </is>
@@ -928,7 +901,7 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="15.42578125" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="14.28515625" bestFit="1" customWidth="1" min="2" max="2"/>

</xml_diff>

<commit_message>
Created simple account window and fixed some minor functionality in the transactions code.
</commit_message>
<xml_diff>
--- a/transactionsSpreadsheet.xlsx
+++ b/transactionsSpreadsheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-28920" yWindow="2985" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -46,11 +46,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,59 +429,73 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col width="16.5703125" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="16.5703125" customWidth="1" min="2" max="2"/>
-    <col width="9.5703125" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="38.28515625" customWidth="1" style="1" min="5" max="5"/>
+    <col width="18.85546875" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="26.5703125" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="16.5703125" customWidth="1" min="3" max="3"/>
+    <col width="10.42578125" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="38.28515625" customWidth="1" style="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>bought new bike</t>
+          <t>Description</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>US Bank Checking</t>
+          <t>Category</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>15000.29</t>
+          <t>Account</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>01-01-2023</t>
+          <t>Amount</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Memo</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>new car</t>
+          <t>bought new bike</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>Recreational</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>US Bank Checking</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>80000</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
+      <c r="D2" t="n">
+        <v>15000.29</v>
+      </c>
+      <c r="E2" t="inlineStr">
         <is>
           <t>01-01-2023</t>
         </is>
@@ -489,20 +504,23 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>new car 2</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>Transportation</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>US Bank Checking</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>90000</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
+      <c r="D3" t="n">
+        <v>80000</v>
+      </c>
+      <c r="E3" t="inlineStr">
         <is>
           <t>01-01-2023</t>
         </is>
@@ -511,20 +529,23 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>mortgage</t>
+          <t>new car 2</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>Recreational</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>US Bank Checking</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>2000</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
+      <c r="D4" t="n">
+        <v>90000</v>
+      </c>
+      <c r="E4" t="inlineStr">
         <is>
           <t>01-01-2023</t>
         </is>
@@ -533,20 +554,23 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Cell Phone</t>
+          <t>mortgage</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>US Bank Savings</t>
+          <t>Housing</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>699.99</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
+          <t>US Bank Checking</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E5" t="inlineStr">
         <is>
           <t>01-01-2023</t>
         </is>
@@ -555,20 +579,23 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Lawn Mower</t>
+          <t>Cell Phone</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Cash in wallet</t>
+          <t>Utilities</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>459.79</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
+          <t>US Bank Savings</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>699.99</v>
+      </c>
+      <c r="E6" t="inlineStr">
         <is>
           <t>01-01-2023</t>
         </is>
@@ -577,108 +604,115 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>New windows</t>
+          <t>Lawn Mower</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>US Bank Checking</t>
+          <t>Household Maintenance</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>33575.84</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>01-01-2023</t>
-        </is>
+          <t>Cash in wallet</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>459.79</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Finally got my new windows!</t>
+          <t>01-01-2023</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Tires for 4Runner</t>
+          <t>New windows</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>US Bank Savings</t>
+          <t>Home Improvement</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1534.34</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>01-01-2023</t>
-        </is>
+          <t>US Bank Checking</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>33575.84</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>35" tires!!</t>
+          <t>01-01-2023</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Finally got my new windows!</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Lift for 4runner</t>
+          <t>Tires for 4Runner</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>US Bank Checking</t>
+          <t>Transportation Maintenance</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>6387.12</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>01-01-2023</t>
-        </is>
+          <t>US Bank Savings</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>1534.34</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>3" lift, Check!!</t>
+          <t>01-01-2023</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>35" tires!!</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Checking for Scroll</t>
+          <t>Lift for 4runner</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
+          <t>Recreational</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
           <t>US Bank Checking</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>.01</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>01-01-2023</t>
-        </is>
+      <c r="D10" t="n">
+        <v>6387.12</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>will this work?</t>
+          <t>01-01-2023</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>3" lift, Check!!</t>
         </is>
       </c>
     </row>
@@ -690,20 +724,23 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
+          <t>Entertainment</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
           <t>US Bank Savings</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>235.69</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>01-01-2023</t>
-        </is>
+      <c r="D11" t="n">
+        <v>235.69</v>
       </c>
       <c r="E11" t="inlineStr">
+        <is>
+          <t>01-01-2023</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
         <is>
           <t>Music!!!</t>
         </is>
@@ -717,20 +754,23 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
+          <t>Recreational</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
           <t>US Bank Savings</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>350.68</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>01-01-2023</t>
-        </is>
+      <c r="D12" t="n">
+        <v>350.68</v>
       </c>
       <c r="E12" t="inlineStr">
+        <is>
+          <t>01-01-2023</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
         <is>
           <t>Bang, Bang</t>
         </is>
@@ -744,15 +784,18 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
+          <t>Business Expenses</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
           <t>US Bank Checking</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>608.79</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
+      <c r="D13" t="n">
+        <v>608.79</v>
+      </c>
+      <c r="E13" t="inlineStr">
         <is>
           <t>01-01-2023</t>
         </is>
@@ -761,127 +804,117 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Powerwheel for Lucas</t>
+          <t>New computer</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
+          <t>Business Expenses</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
           <t>US Bank Checking</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>348.46</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>01-01-2023</t>
-        </is>
+      <c r="D14" t="n">
+        <v>2300.98</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Love that kid!!</t>
+          <t>01-01-2023</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Very powerfull</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>New computer</t>
+          <t>Notebooks for work</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
+          <t>Business Expenses</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
           <t>US Bank Checking</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>2300.98</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>01-01-2023</t>
-        </is>
+      <c r="D15" t="n">
+        <v>18.59</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Very powerfull</t>
+          <t>03-24-2023</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Gotta keep your notes!</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Tire for dirtbike</t>
+          <t>1456156</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
+          <t>Recreational</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
           <t>US Bank Checking</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>97.87</t>
-        </is>
-      </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>01-01-2023</t>
+          <t>1.23</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>04-03-2023</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>New bib for tire</t>
+          <t>fgsfg</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>US Bank Checking</t>
+          <t>Household Maintenance</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>120.35</t>
+          <t>Cash</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>01-01-2023</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Notebooks for work</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>US Bank Checking</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>18.59</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>03-24-2023</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>Gotta keep your notes!</t>
-        </is>
-      </c>
+          <t>1.23</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>04-03-2023</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -895,17 +928,17 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col width="15.42578125" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="22.28515625" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="14.28515625" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="8.85546875" customWidth="1" min="3" max="3"/>
+    <col width="18.140625" bestFit="1" customWidth="1" style="2" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -919,6 +952,11 @@
           <t>Type of Account</t>
         </is>
       </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Amount in Account</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -931,29 +969,98 @@
           <t>Checking</t>
         </is>
       </c>
+      <c r="C2" s="2" t="n">
+        <v>5387.89</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>US Bank Savings</t>
+          <t>Wellsfargo Bank Checking</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Savings</t>
-        </is>
+          <t>Checking</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>3045.78</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>America Credit Union</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Checking</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>2897.87</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Wellsfargo Bank Checking</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Savings</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>America Credit Union</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Savings</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>2987.45</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>US Bank Savings</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Savings</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>8674.559999999999</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
           <t>Cash in wallet</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B8" t="inlineStr">
         <is>
           <t>Cash</t>
         </is>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>250.89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Replaced QTableWidget with QTableView for the Transaction Table. Connected Transaction Database to Transaction Tab and removed the filter/clear filter buttons. Made the Transaction Filter Text box signal when it changes to initiate filtering of table. Connect editing of Transaction table to update database.
</commit_message>
<xml_diff>
--- a/transactionsSpreadsheet.xlsx
+++ b/transactionsSpreadsheet.xlsx
@@ -436,13 +436,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A676" sqref="A17:XFD676"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
     <col width="18.88671875" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="26.5546875" bestFit="1" customWidth="1" min="2" max="2"/>
@@ -841,7 +841,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Notebooks for work</t>
+          <t>test</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -871,7 +871,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>1456156</t>
+          <t>test2</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -894,66 +894,6 @@
           <t>04-03-2023</t>
         </is>
       </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>ads</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Business Expenses</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Cash</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>2.00</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>04-10-2023</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>asd</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>asdsdasdsa</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Business Expenses</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Checking</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>532.00</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>04-10-2023</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -973,7 +913,7 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
     <col width="22.33203125" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="14.33203125" bestFit="1" customWidth="1" min="2" max="2"/>
@@ -1120,7 +1060,7 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
     <col width="26.5546875" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="25.33203125" customWidth="1" min="2" max="2"/>

</xml_diff>